<commit_message>
1. Add excel report and page display 2. filter out buggy value
</commit_message>
<xml_diff>
--- a/Dahs2BlazorApp/wwwroot/ReportTemplate/DailyReport.xlsx
+++ b/Dahs2BlazorApp/wwwroot/ReportTemplate/DailyReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\CPMS2\Dahs2BlazorApp\ExcelReport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\CPMS2\Dahs2BlazorApp\wwwroot\ReportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7317A42-B638-4A7D-89F0-09988666C9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83BD43B-6EF2-4FEB-837C-349E668D119E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{21EA2AD6-FE5B-42AD-AE04-C86E3020F209}"/>
+    <workbookView xWindow="5666" yWindow="11554" windowWidth="25860" windowHeight="13055" xr2:uid="{21EA2AD6-FE5B-42AD-AE04-C86E3020F209}"/>
   </bookViews>
   <sheets>
     <sheet name="M01" sheetId="1" r:id="rId1"/>
@@ -841,7 +841,7 @@
   <dimension ref="B1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="O4" sqref="O4:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
1. Five minute value is actual reading. 2. Hour is average or diff 3. Fix excel digital format.
</commit_message>
<xml_diff>
--- a/Dahs2BlazorApp/wwwroot/ReportTemplate/DailyReport.xlsx
+++ b/Dahs2BlazorApp/wwwroot/ReportTemplate/DailyReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\CPMS2\Dahs2BlazorApp\wwwroot\ReportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E968FF1-100D-43F2-886E-11A80BEA2736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7B1C4C-D2BA-499B-80E2-D0CF36CBD807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{21EA2AD6-FE5B-42AD-AE04-C86E3020F209}"/>
+    <workbookView xWindow="6557" yWindow="2769" windowWidth="26357" windowHeight="13054" xr2:uid="{21EA2AD6-FE5B-42AD-AE04-C86E3020F209}"/>
   </bookViews>
   <sheets>
     <sheet name="M01" sheetId="1" r:id="rId1"/>
@@ -284,6 +284,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -493,7 +496,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -547,6 +550,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0897718-5C20-4BD0-A9E4-4BC4D614F1DD}">
   <dimension ref="B1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
@@ -1619,21 +1628,21 @@
       <c r="B36" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="9"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="19"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B37" s="8" t="s">

</xml_diff>